<commit_message>
Ellipse_PS - Update Test Case  OK
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111ENGINNERING/Engineering_Ingegneria_Informatica_S.p.A/Ellipse_PS/2.7.0/report-checklist.xlsx
+++ b/GATEWAY/S1#111ENGINNERING/Engineering_Ingegneria_Informatica_S.p.A/Ellipse_PS/2.7.0/report-checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://engit-my.sharepoint.com/personal/cristiano_avella_eng_it/Documents/Documenti/GitHub/it-fse-accreditamento/GATEWAY/S1#111ENGINNERING/Engineering_Ingegneria_Informatica_S.p.A/Ellipse_PS/2.7.0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="34" documentId="8_{5C1BE210-EF7F-4D01-8879-4722001918C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{757EA181-9D65-4FE1-8CAF-769AC19D4A20}"/>
+  <xr:revisionPtr revIDLastSave="56" documentId="8_{5C1BE210-EF7F-4D01-8879-4722001918C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3F907C07-E38E-41A6-8C81-2B27B964F047}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="5" r:id="rId1"/>
@@ -1705,40 +1705,40 @@
     <t>2023-03-08T14:33:56Z</t>
   </si>
   <si>
-    <t>debab80fbaba5990</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.1.554bc96737cb087a135c9b0770580e1440c992adea27f8cffaf148bb208b11cb.8d4d4878d3^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-03-23T17:50:38Z</t>
-  </si>
-  <si>
-    <t>ebe5c6e770293625</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.1.0bd90d34f14c0eccff8f33c33ae223db4edf4644f0917873e751aae1854b2e18.64d443f5ca^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-03-23T17:58:25Z</t>
-  </si>
-  <si>
-    <t>869269a591fea43b</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.1.822a6be25dec3144fe15048ced700c2ee3c2b87fdd9387fd4dcaffe71818f811.480a0ee8d2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-03-24T12:48:55Z</t>
-  </si>
-  <si>
-    <t>4d4d0d5929d4a7f3</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.1.41f0ccb2b77166e5edbb1c49bddcdb15e018a0a6490c6dbcbfd9295c9970b44e.bda781f0f1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-03-24T15:53:57Z</t>
+    <t>569d6d66fc64555c</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.1.5dc64e2b66d2b69ca5c389e2212c9c02c408118afe923dce627055bb2cd4d610.9760adab63^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-03-30T11:10:37Z</t>
+  </si>
+  <si>
+    <t>aa60e396356b12cd</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.1.a60ce5e28ac814f041150b320c6a9342dc95d808d5a54e4b5db715de0ae8a347.c7eba00609^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-03-30T11:35:57Z</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.1.cd6dd70ef2ba31a9918398c0da847da1babf052bbfe6e6465210a3066084804b.740b436dd5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>0a62db91925748e9</t>
+  </si>
+  <si>
+    <t>2023-03-30T11:44:51Z</t>
+  </si>
+  <si>
+    <t>3be613f4f40af162</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.1.fa2c9515f28a87f97dac344e5b9f3cd5f35b65c5a4d411fa5c8d9bf3bd493cf8.8f81cfb81e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-03-30T13:17:19Z</t>
   </si>
 </sst>
 </file>
@@ -3898,10 +3898,10 @@
   <dimension ref="A1:T992"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="K131" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="D31" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="F34" sqref="F34"/>
+      <selection pane="bottomRight" activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4891,7 +4891,7 @@
         <v>94</v>
       </c>
       <c r="F31" s="42">
-        <v>45008.743495370371</v>
+        <v>45015.46570601852</v>
       </c>
       <c r="G31" s="43" t="s">
         <v>412</v>
@@ -4935,7 +4935,7 @@
         <v>97</v>
       </c>
       <c r="F32" s="42">
-        <v>45008.748900462961</v>
+        <v>45015.483298611114</v>
       </c>
       <c r="G32" s="43" t="s">
         <v>415</v>
@@ -4979,16 +4979,16 @@
         <v>99</v>
       </c>
       <c r="F33" s="42">
-        <v>45009.53396990741</v>
+        <v>45015.489479166667</v>
       </c>
       <c r="G33" s="43" t="s">
         <v>418</v>
       </c>
       <c r="H33" s="43" t="s">
+        <v>417</v>
+      </c>
+      <c r="I33" s="43" t="s">
         <v>416</v>
-      </c>
-      <c r="I33" s="43" t="s">
-        <v>417</v>
       </c>
       <c r="J33" s="44" t="s">
         <v>95</v>
@@ -5023,7 +5023,7 @@
         <v>101</v>
       </c>
       <c r="F34" s="42">
-        <v>45009.662465277775</v>
+        <v>45015.55369212963</v>
       </c>
       <c r="G34" s="43" t="s">
         <v>421</v>
@@ -5682,7 +5682,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="52" spans="1:20" ht="115.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:20" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="31">
         <v>51</v>
       </c>
@@ -25820,21 +25820,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101004DE490683678E84AABC70C83AF04A849" ma:contentTypeVersion="5" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="d87ba405330fe1fd4ebca86e6510eeed">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6b66a4e9-493a-4f5b-bd90-2639920d41ca" xmlns:ns3="581feeb0-3f31-43f8-b205-816acbb15e2f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7a33c0baab722015f1fb37e23302defe" ns2:_="" ns3:_="">
     <xsd:import namespace="6b66a4e9-493a-4f5b-bd90-2639920d41ca"/>
@@ -26005,26 +25990,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAAC13FE-B745-460A-BC76-FAEE62F3EBA1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3F02EBF-A415-4FB6-A4E4-A6920890B7C4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FFD964D2-2703-4697-A7AA-1232AB3EB4A9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -26043,6 +26024,25 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3F02EBF-A415-4FB6-A4E4-A6920890B7C4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAAC13FE-B745-460A-BC76-FAEE62F3EBA1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{e0793d39-0939-496d-b129-198edd916feb}" enabled="0" method="" siteId="{e0793d39-0939-496d-b129-198edd916feb}" removed="1"/>

</xml_diff>